<commit_message>
Required modifications are done to achieve expected actions
</commit_message>
<xml_diff>
--- a/test_data/Test Data.xlsx
+++ b/test_data/Test Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="57">
   <si>
     <t>Test Case No.</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Sauce Labs Fleece Jacket, Sauce Labs Bolt T-Shirt</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket</t>
   </si>
   <si>
     <t>John</t>
@@ -190,7 +193,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,12 +211,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -252,23 +249,23 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -582,8 +579,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="25.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="7" width="21.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -598,7 +595,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
@@ -637,7 +634,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>20</v>
@@ -645,10 +642,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -659,13 +656,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>20</v>
@@ -673,10 +670,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="1" t="s">
@@ -685,10 +682,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -699,13 +696,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>20</v>
@@ -713,7 +710,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -740,12 +737,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="22.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="7" width="19.719285714285714" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="7" width="66.57642857142856" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="7" width="42.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="7" width="14.862142857142858" customWidth="1" bestFit="1"/>
@@ -764,22 +761,22 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -796,22 +793,22 @@
       <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <v>14182</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -828,22 +825,22 @@
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>17866</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -860,31 +857,31 @@
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="5">
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="4">
         <v>62236</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -892,31 +889,31 @@
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="H5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="4">
         <v>30240</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -924,57 +921,57 @@
       <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="3" t="s">
+      <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="5">
+      <c r="H6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="4">
         <v>24309</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="5">
+      <c r="F7" s="5"/>
+      <c r="G7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="4">
         <v>87034</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -982,28 +979,28 @@
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="5">
+      <c r="H8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="4">
         <v>85223</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
@@ -1014,26 +1011,26 @@
       <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="5">
+      <c r="E9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="4">
         <v>31103</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -1042,20 +1039,20 @@
       <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" s="5">
+      <c r="H10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="4">
         <v>73038</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>